<commit_message>
review after first submission to James
</commit_message>
<xml_diff>
--- a/Summary - Indicator availability for RC countries.xlsx
+++ b/Summary - Indicator availability for RC countries.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitednations-my.sharepoint.com/personal/gonzalezmorales_un_org/Documents/UNCT - Toolkit/Data availability/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.GonzalezMorales\OneDrive - United Nations\UNCT - Toolkit\Data availability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{EB8E6909-BD1D-4045-A028-5EBA58FD66B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{9494C668-FC6B-48A6-BC51-E121F376F011}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{EB8E6909-BD1D-4045-A028-5EBA58FD66B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E4DEA71C-C6EA-4995-8570-D0141AAACD57}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{EBCAA7D1-E953-4234-B5E2-04FD95F11795}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="2" xr2:uid="{EBCAA7D1-E953-4234-B5E2-04FD95F11795}"/>
   </bookViews>
   <sheets>
     <sheet name="RC countries - Tiers 1 and 2" sheetId="1" r:id="rId1"/>
     <sheet name="Indicators - Tiers 1 and 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Poverty - latest year available" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="Poverty - latest year available" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1972,8 +1973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F6DDCB-499C-464D-A10D-6D5C3B58F6B7}">
   <dimension ref="A1:L131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6193,7 +6194,7 @@
   <dimension ref="A1:I155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D3" sqref="D3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10705,11 +10706,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9304205-4745-49F2-9D2C-F9268C728CE6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794B12D4-505C-4DA5-B5A4-BF2516ADD42D}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>